<commit_message>
fixed broken excel reference
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Desktop\GitHub\spl-schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9EA577-DC36-4877-AFFC-DE3194AA7525}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80EE7D9-4AEE-4028-B8BF-73BA57282A2C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{CB2829CA-F4A0-41C5-B1C7-1ACBB28571D8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{CB2829CA-F4A0-41C5-B1C7-1ACBB28571D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Preferences" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,6 @@
     <sheet name="Dictionary" sheetId="2" r:id="rId4"/>
     <sheet name="Keys" sheetId="4" r:id="rId5"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId6"/>
-  </externalReferences>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -967,448 +964,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Preferences"/>
-      <sheetName val="Dictionary"/>
-      <sheetName val="Sheet1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="11">
-          <cell r="C11" t="str">
-            <v>P</v>
-          </cell>
-          <cell r="D11" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="E11" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="F11" t="str">
-            <v>U</v>
-          </cell>
-          <cell r="G11" t="str">
-            <v>U</v>
-          </cell>
-          <cell r="H11" t="str">
-            <v>U</v>
-          </cell>
-          <cell r="I11" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="J11" t="str">
-            <v>U</v>
-          </cell>
-          <cell r="K11" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="L11" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="M11" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="N11" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="O11" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="P11" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="Q11" t="str">
-            <v>U</v>
-          </cell>
-          <cell r="R11" t="str">
-            <v>U</v>
-          </cell>
-          <cell r="S11" t="str">
-            <v>U</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="C12" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="D12" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="E12" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="F12" t="str">
-            <v>P</v>
-          </cell>
-          <cell r="G12" t="str">
-            <v>P</v>
-          </cell>
-          <cell r="H12" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="I12" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="J12" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="K12" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="L12" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="M12" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="N12" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="O12" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="P12" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="Q12" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="R12" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="S12" t="str">
-            <v>N</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="C13" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="D13" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="E13" t="str">
-            <v>P</v>
-          </cell>
-          <cell r="F13" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="G13" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="H13" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="I13" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="J13" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="K13" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="L13" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="M13" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="N13" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="O13" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="P13" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="Q13" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="R13" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="S13" t="str">
-            <v>C</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="C14" t="str">
-            <v>P</v>
-          </cell>
-          <cell r="D14" t="str">
-            <v>P</v>
-          </cell>
-          <cell r="E14" t="str">
-            <v>P</v>
-          </cell>
-          <cell r="F14" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="G14" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="H14" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="I14" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="J14" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="K14" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="L14" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="M14" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="N14" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="O14" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="P14" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="Q14" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="R14" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="S14" t="str">
-            <v>C</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="C15" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="D15" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="E15" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="F15" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="G15" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="H15" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="I15" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="J15" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="K15" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="L15" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="M15" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="N15" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="O15" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="P15" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="Q15" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="R15" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="S15" t="str">
-            <v>C</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="C16" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="D16" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="E16" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="F16" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="G16" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="H16" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="I16" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="J16" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="K16" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="L16" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="M16" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="N16" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="O16" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="P16" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="Q16" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="R16" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="S16" t="str">
-            <v>C</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="C17" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="D17" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="E17" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="F17" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="G17" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="H17" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="I17" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="J17" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="K17" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="L17" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="M17" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="N17" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="O17" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="P17" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="Q17" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="R17" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="S17" t="str">
-            <v>N</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="C18" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="D18" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="E18" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="F18" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="G18" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="H18" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="I18" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="J18" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="K18" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="L18" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="M18" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="N18" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="O18" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="P18" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="Q18" t="str">
-            <v>N</v>
-          </cell>
-          <cell r="R18" t="str">
-            <v>C</v>
-          </cell>
-          <cell r="S18" t="str">
-            <v>C</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1709,7 +1264,7 @@
   <dimension ref="A1:T38"/>
   <sheetViews>
     <sheetView zoomScale="66" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2569,569 +2124,569 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EF632EB-8448-49AC-B390-FB4C681997FA}">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1">
-        <f>IF([1]Preferences!C11="P",1,(IF([1]Preferences!C11="N",0,(IF([1]Preferences!C11="U",-1,(IF([1]Preferences!C11="C",-1000)))))))</f>
+        <f>IF(Preferences!C11="P",1,(IF(Preferences!C11="N",0,(IF(Preferences!C11="U",-1,(IF(Preferences!C11="C",-1000)))))))</f>
         <v>1</v>
       </c>
       <c r="B1">
-        <f>IF([1]Preferences!D11="P",1,(IF([1]Preferences!D11="N",0,(IF([1]Preferences!D11="U",-1,(IF([1]Preferences!D11="C",-1000)))))))</f>
+        <f>IF(Preferences!D11="P",1,(IF(Preferences!D11="N",0,(IF(Preferences!D11="U",-1,(IF(Preferences!D11="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="C1">
-        <f>IF([1]Preferences!E11="P",1,(IF([1]Preferences!E11="N",0,(IF([1]Preferences!E11="U",-1,(IF([1]Preferences!E11="C",-1000)))))))</f>
+        <f>IF(Preferences!E11="P",1,(IF(Preferences!E11="N",0,(IF(Preferences!E11="U",-1,(IF(Preferences!E11="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="D1">
-        <f>IF([1]Preferences!F11="P",1,(IF([1]Preferences!F11="N",0,(IF([1]Preferences!F11="U",-1,(IF([1]Preferences!F11="C",-1000)))))))</f>
+        <f>IF(Preferences!F11="P",1,(IF(Preferences!F11="N",0,(IF(Preferences!F11="U",-1,(IF(Preferences!F11="C",-1000)))))))</f>
         <v>-1</v>
       </c>
       <c r="E1">
-        <f>IF([1]Preferences!G11="P",1,(IF([1]Preferences!G11="N",0,(IF([1]Preferences!G11="U",-1,(IF([1]Preferences!G11="C",-1000)))))))</f>
+        <f>IF(Preferences!G11="P",1,(IF(Preferences!G11="N",0,(IF(Preferences!G11="U",-1,(IF(Preferences!G11="C",-1000)))))))</f>
         <v>-1</v>
       </c>
       <c r="F1">
-        <f>IF([1]Preferences!H11="P",1,(IF([1]Preferences!H11="N",0,(IF([1]Preferences!H11="U",-1,(IF([1]Preferences!H11="C",-1000)))))))</f>
+        <f>IF(Preferences!H11="P",1,(IF(Preferences!H11="N",0,(IF(Preferences!H11="U",-1,(IF(Preferences!H11="C",-1000)))))))</f>
         <v>-1</v>
       </c>
       <c r="G1">
-        <f>IF([1]Preferences!I11="P",1,(IF([1]Preferences!I11="N",0,(IF([1]Preferences!I11="U",-1,(IF([1]Preferences!I11="C",-1000)))))))</f>
+        <f>IF(Preferences!I11="P",1,(IF(Preferences!I11="N",0,(IF(Preferences!I11="U",-1,(IF(Preferences!I11="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="H1">
-        <f>IF([1]Preferences!J11="P",1,(IF([1]Preferences!J11="N",0,(IF([1]Preferences!J11="U",-1,(IF([1]Preferences!J11="C",-1000)))))))</f>
+        <f>IF(Preferences!J11="P",1,(IF(Preferences!J11="N",0,(IF(Preferences!J11="U",-1,(IF(Preferences!J11="C",-1000)))))))</f>
         <v>-1</v>
       </c>
       <c r="I1">
-        <f>IF([1]Preferences!K11="P",1,(IF([1]Preferences!K11="N",0,(IF([1]Preferences!K11="U",-1,(IF([1]Preferences!K11="C",-1000)))))))</f>
+        <f>IF(Preferences!K11="P",1,(IF(Preferences!K11="N",0,(IF(Preferences!K11="U",-1,(IF(Preferences!K11="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="J1">
-        <f>IF([1]Preferences!L11="P",1,(IF([1]Preferences!L11="N",0,(IF([1]Preferences!L11="U",-1,(IF([1]Preferences!L11="C",-1000)))))))</f>
+        <f>IF(Preferences!L11="P",1,(IF(Preferences!L11="N",0,(IF(Preferences!L11="U",-1,(IF(Preferences!L11="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="K1">
-        <f>IF([1]Preferences!M11="P",1,(IF([1]Preferences!M11="N",0,(IF([1]Preferences!M11="U",-1,(IF([1]Preferences!M11="C",-1000)))))))</f>
+        <f>IF(Preferences!M11="P",1,(IF(Preferences!M11="N",0,(IF(Preferences!M11="U",-1,(IF(Preferences!M11="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="L1">
-        <f>IF([1]Preferences!N11="P",1,(IF([1]Preferences!N11="N",0,(IF([1]Preferences!N11="U",-1,(IF([1]Preferences!N11="C",-1000)))))))</f>
+        <f>IF(Preferences!N11="P",1,(IF(Preferences!N11="N",0,(IF(Preferences!N11="U",-1,(IF(Preferences!N11="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="M1">
-        <f>IF([1]Preferences!O11="P",1,(IF([1]Preferences!O11="N",0,(IF([1]Preferences!O11="U",-1,(IF([1]Preferences!O11="C",-1000)))))))</f>
+        <f>IF(Preferences!O11="P",1,(IF(Preferences!O11="N",0,(IF(Preferences!O11="U",-1,(IF(Preferences!O11="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="N1">
-        <f>IF([1]Preferences!P11="P",1,(IF([1]Preferences!P11="N",0,(IF([1]Preferences!P11="U",-1,(IF([1]Preferences!P11="C",-1000)))))))</f>
+        <f>IF(Preferences!P11="P",1,(IF(Preferences!P11="N",0,(IF(Preferences!P11="U",-1,(IF(Preferences!P11="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="O1">
-        <f>IF([1]Preferences!Q11="P",1,(IF([1]Preferences!Q11="N",0,(IF([1]Preferences!Q11="U",-1,(IF([1]Preferences!Q11="C",-1000)))))))</f>
+        <f>IF(Preferences!Q11="P",1,(IF(Preferences!Q11="N",0,(IF(Preferences!Q11="U",-1,(IF(Preferences!Q11="C",-1000)))))))</f>
         <v>-1</v>
       </c>
       <c r="P1">
-        <f>IF([1]Preferences!R11="P",1,(IF([1]Preferences!R11="N",0,(IF([1]Preferences!R11="U",-1,(IF([1]Preferences!R11="C",-1000)))))))</f>
+        <f>IF(Preferences!R11="P",1,(IF(Preferences!R11="N",0,(IF(Preferences!R11="U",-1,(IF(Preferences!R11="C",-1000)))))))</f>
         <v>-1</v>
       </c>
       <c r="Q1">
-        <f>IF([1]Preferences!S11="P",1,(IF([1]Preferences!S11="N",0,(IF([1]Preferences!S11="U",-1,(IF([1]Preferences!S11="C",-1000)))))))</f>
+        <f>IF(Preferences!S11="P",1,(IF(Preferences!S11="N",0,(IF(Preferences!S11="U",-1,(IF(Preferences!S11="C",-1000)))))))</f>
         <v>-1</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
-        <f>IF([1]Preferences!C12="P",1,(IF([1]Preferences!C12="N",0,(IF([1]Preferences!C12="U",-1,(IF([1]Preferences!C12="C",-1000)))))))</f>
+        <f>IF(Preferences!C12="P",1,(IF(Preferences!C12="N",0,(IF(Preferences!C12="U",-1,(IF(Preferences!C12="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="B2">
-        <f>IF([1]Preferences!D12="P",1,(IF([1]Preferences!D12="N",0,(IF([1]Preferences!D12="U",-1,(IF([1]Preferences!D12="C",-1000)))))))</f>
+        <f>IF(Preferences!D12="P",1,(IF(Preferences!D12="N",0,(IF(Preferences!D12="U",-1,(IF(Preferences!D12="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="C2">
-        <f>IF([1]Preferences!E12="P",1,(IF([1]Preferences!E12="N",0,(IF([1]Preferences!E12="U",-1,(IF([1]Preferences!E12="C",-1000)))))))</f>
+        <f>IF(Preferences!E12="P",1,(IF(Preferences!E12="N",0,(IF(Preferences!E12="U",-1,(IF(Preferences!E12="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="D2">
-        <f>IF([1]Preferences!F12="P",1,(IF([1]Preferences!F12="N",0,(IF([1]Preferences!F12="U",-1,(IF([1]Preferences!F12="C",-1000)))))))</f>
+        <f>IF(Preferences!F12="P",1,(IF(Preferences!F12="N",0,(IF(Preferences!F12="U",-1,(IF(Preferences!F12="C",-1000)))))))</f>
         <v>1</v>
       </c>
       <c r="E2">
-        <f>IF([1]Preferences!G12="P",1,(IF([1]Preferences!G12="N",0,(IF([1]Preferences!G12="U",-1,(IF([1]Preferences!G12="C",-1000)))))))</f>
+        <f>IF(Preferences!G12="P",1,(IF(Preferences!G12="N",0,(IF(Preferences!G12="U",-1,(IF(Preferences!G12="C",-1000)))))))</f>
         <v>1</v>
       </c>
       <c r="F2">
-        <f>IF([1]Preferences!H12="P",1,(IF([1]Preferences!H12="N",0,(IF([1]Preferences!H12="U",-1,(IF([1]Preferences!H12="C",-1000)))))))</f>
+        <f>IF(Preferences!H12="P",1,(IF(Preferences!H12="N",0,(IF(Preferences!H12="U",-1,(IF(Preferences!H12="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="G2">
-        <f>IF([1]Preferences!I12="P",1,(IF([1]Preferences!I12="N",0,(IF([1]Preferences!I12="U",-1,(IF([1]Preferences!I12="C",-1000)))))))</f>
+        <f>IF(Preferences!I12="P",1,(IF(Preferences!I12="N",0,(IF(Preferences!I12="U",-1,(IF(Preferences!I12="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="H2">
-        <f>IF([1]Preferences!J12="P",1,(IF([1]Preferences!J12="N",0,(IF([1]Preferences!J12="U",-1,(IF([1]Preferences!J12="C",-1000)))))))</f>
+        <f>IF(Preferences!J12="P",1,(IF(Preferences!J12="N",0,(IF(Preferences!J12="U",-1,(IF(Preferences!J12="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="I2">
-        <f>IF([1]Preferences!K12="P",1,(IF([1]Preferences!K12="N",0,(IF([1]Preferences!K12="U",-1,(IF([1]Preferences!K12="C",-1000)))))))</f>
+        <f>IF(Preferences!K12="P",1,(IF(Preferences!K12="N",0,(IF(Preferences!K12="U",-1,(IF(Preferences!K12="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="J2">
-        <f>IF([1]Preferences!L12="P",1,(IF([1]Preferences!L12="N",0,(IF([1]Preferences!L12="U",-1,(IF([1]Preferences!L12="C",-1000)))))))</f>
+        <f>IF(Preferences!L12="P",1,(IF(Preferences!L12="N",0,(IF(Preferences!L12="U",-1,(IF(Preferences!L12="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="K2">
-        <f>IF([1]Preferences!M12="P",1,(IF([1]Preferences!M12="N",0,(IF([1]Preferences!M12="U",-1,(IF([1]Preferences!M12="C",-1000)))))))</f>
+        <f>IF(Preferences!M12="P",1,(IF(Preferences!M12="N",0,(IF(Preferences!M12="U",-1,(IF(Preferences!M12="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="L2">
-        <f>IF([1]Preferences!N12="P",1,(IF([1]Preferences!N12="N",0,(IF([1]Preferences!N12="U",-1,(IF([1]Preferences!N12="C",-1000)))))))</f>
+        <f>IF(Preferences!N12="P",1,(IF(Preferences!N12="N",0,(IF(Preferences!N12="U",-1,(IF(Preferences!N12="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="M2">
-        <f>IF([1]Preferences!O12="P",1,(IF([1]Preferences!O12="N",0,(IF([1]Preferences!O12="U",-1,(IF([1]Preferences!O12="C",-1000)))))))</f>
+        <f>IF(Preferences!O12="P",1,(IF(Preferences!O12="N",0,(IF(Preferences!O12="U",-1,(IF(Preferences!O12="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="N2">
-        <f>IF([1]Preferences!P12="P",1,(IF([1]Preferences!P12="N",0,(IF([1]Preferences!P12="U",-1,(IF([1]Preferences!P12="C",-1000)))))))</f>
+        <f>IF(Preferences!P12="P",1,(IF(Preferences!P12="N",0,(IF(Preferences!P12="U",-1,(IF(Preferences!P12="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="O2">
-        <f>IF([1]Preferences!Q12="P",1,(IF([1]Preferences!Q12="N",0,(IF([1]Preferences!Q12="U",-1,(IF([1]Preferences!Q12="C",-1000)))))))</f>
+        <f>IF(Preferences!Q12="P",1,(IF(Preferences!Q12="N",0,(IF(Preferences!Q12="U",-1,(IF(Preferences!Q12="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="P2">
-        <f>IF([1]Preferences!R12="P",1,(IF([1]Preferences!R12="N",0,(IF([1]Preferences!R12="U",-1,(IF([1]Preferences!R12="C",-1000)))))))</f>
+        <f>IF(Preferences!R12="P",1,(IF(Preferences!R12="N",0,(IF(Preferences!R12="U",-1,(IF(Preferences!R12="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="Q2">
-        <f>IF([1]Preferences!S12="P",1,(IF([1]Preferences!S12="N",0,(IF([1]Preferences!S12="U",-1,(IF([1]Preferences!S12="C",-1000)))))))</f>
+        <f>IF(Preferences!S12="P",1,(IF(Preferences!S12="N",0,(IF(Preferences!S12="U",-1,(IF(Preferences!S12="C",-1000)))))))</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
-        <f>IF([1]Preferences!C13="P",1,(IF([1]Preferences!C13="N",0,(IF([1]Preferences!C13="U",-1,(IF([1]Preferences!C13="C",-1000)))))))</f>
+        <f>IF(Preferences!C13="P",1,(IF(Preferences!C13="N",0,(IF(Preferences!C13="U",-1,(IF(Preferences!C13="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="B3">
-        <f>IF([1]Preferences!D13="P",1,(IF([1]Preferences!D13="N",0,(IF([1]Preferences!D13="U",-1,(IF([1]Preferences!D13="C",-1000)))))))</f>
+        <f>IF(Preferences!D13="P",1,(IF(Preferences!D13="N",0,(IF(Preferences!D13="U",-1,(IF(Preferences!D13="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="C3">
-        <f>IF([1]Preferences!E13="P",1,(IF([1]Preferences!E13="N",0,(IF([1]Preferences!E13="U",-1,(IF([1]Preferences!E13="C",-1000)))))))</f>
+        <f>IF(Preferences!E13="P",1,(IF(Preferences!E13="N",0,(IF(Preferences!E13="U",-1,(IF(Preferences!E13="C",-1000)))))))</f>
         <v>1</v>
       </c>
       <c r="D3">
-        <f>IF([1]Preferences!F13="P",1,(IF([1]Preferences!F13="N",0,(IF([1]Preferences!F13="U",-1,(IF([1]Preferences!F13="C",-1000)))))))</f>
+        <f>IF(Preferences!F13="P",1,(IF(Preferences!F13="N",0,(IF(Preferences!F13="U",-1,(IF(Preferences!F13="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="E3">
-        <f>IF([1]Preferences!G13="P",1,(IF([1]Preferences!G13="N",0,(IF([1]Preferences!G13="U",-1,(IF([1]Preferences!G13="C",-1000)))))))</f>
+        <f>IF(Preferences!G13="P",1,(IF(Preferences!G13="N",0,(IF(Preferences!G13="U",-1,(IF(Preferences!G13="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="F3">
-        <f>IF([1]Preferences!H13="P",1,(IF([1]Preferences!H13="N",0,(IF([1]Preferences!H13="U",-1,(IF([1]Preferences!H13="C",-1000)))))))</f>
+        <f>IF(Preferences!H13="P",1,(IF(Preferences!H13="N",0,(IF(Preferences!H13="U",-1,(IF(Preferences!H13="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="G3">
-        <f>IF([1]Preferences!I13="P",1,(IF([1]Preferences!I13="N",0,(IF([1]Preferences!I13="U",-1,(IF([1]Preferences!I13="C",-1000)))))))</f>
+        <f>IF(Preferences!I13="P",1,(IF(Preferences!I13="N",0,(IF(Preferences!I13="U",-1,(IF(Preferences!I13="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="H3">
-        <f>IF([1]Preferences!J13="P",1,(IF([1]Preferences!J13="N",0,(IF([1]Preferences!J13="U",-1,(IF([1]Preferences!J13="C",-1000)))))))</f>
+        <f>IF(Preferences!J13="P",1,(IF(Preferences!J13="N",0,(IF(Preferences!J13="U",-1,(IF(Preferences!J13="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="I3">
-        <f>IF([1]Preferences!K13="P",1,(IF([1]Preferences!K13="N",0,(IF([1]Preferences!K13="U",-1,(IF([1]Preferences!K13="C",-1000)))))))</f>
+        <f>IF(Preferences!K13="P",1,(IF(Preferences!K13="N",0,(IF(Preferences!K13="U",-1,(IF(Preferences!K13="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="J3">
-        <f>IF([1]Preferences!L13="P",1,(IF([1]Preferences!L13="N",0,(IF([1]Preferences!L13="U",-1,(IF([1]Preferences!L13="C",-1000)))))))</f>
+        <f>IF(Preferences!L13="P",1,(IF(Preferences!L13="N",0,(IF(Preferences!L13="U",-1,(IF(Preferences!L13="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="K3">
-        <f>IF([1]Preferences!M13="P",1,(IF([1]Preferences!M13="N",0,(IF([1]Preferences!M13="U",-1,(IF([1]Preferences!M13="C",-1000)))))))</f>
+        <f>IF(Preferences!M13="P",1,(IF(Preferences!M13="N",0,(IF(Preferences!M13="U",-1,(IF(Preferences!M13="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="L3">
-        <f>IF([1]Preferences!N13="P",1,(IF([1]Preferences!N13="N",0,(IF([1]Preferences!N13="U",-1,(IF([1]Preferences!N13="C",-1000)))))))</f>
+        <f>IF(Preferences!N13="P",1,(IF(Preferences!N13="N",0,(IF(Preferences!N13="U",-1,(IF(Preferences!N13="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="M3">
-        <f>IF([1]Preferences!O13="P",1,(IF([1]Preferences!O13="N",0,(IF([1]Preferences!O13="U",-1,(IF([1]Preferences!O13="C",-1000)))))))</f>
+        <f>IF(Preferences!O13="P",1,(IF(Preferences!O13="N",0,(IF(Preferences!O13="U",-1,(IF(Preferences!O13="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="N3">
-        <f>IF([1]Preferences!P13="P",1,(IF([1]Preferences!P13="N",0,(IF([1]Preferences!P13="U",-1,(IF([1]Preferences!P13="C",-1000)))))))</f>
+        <f>IF(Preferences!P13="P",1,(IF(Preferences!P13="N",0,(IF(Preferences!P13="U",-1,(IF(Preferences!P13="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="O3">
-        <f>IF([1]Preferences!Q13="P",1,(IF([1]Preferences!Q13="N",0,(IF([1]Preferences!Q13="U",-1,(IF([1]Preferences!Q13="C",-1000)))))))</f>
+        <f>IF(Preferences!Q13="P",1,(IF(Preferences!Q13="N",0,(IF(Preferences!Q13="U",-1,(IF(Preferences!Q13="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="P3">
-        <f>IF([1]Preferences!R13="P",1,(IF([1]Preferences!R13="N",0,(IF([1]Preferences!R13="U",-1,(IF([1]Preferences!R13="C",-1000)))))))</f>
+        <f>IF(Preferences!R13="P",1,(IF(Preferences!R13="N",0,(IF(Preferences!R13="U",-1,(IF(Preferences!R13="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="Q3">
-        <f>IF([1]Preferences!S13="P",1,(IF([1]Preferences!S13="N",0,(IF([1]Preferences!S13="U",-1,(IF([1]Preferences!S13="C",-1000)))))))</f>
+        <f>IF(Preferences!S13="P",1,(IF(Preferences!S13="N",0,(IF(Preferences!S13="U",-1,(IF(Preferences!S13="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
-        <f>IF([1]Preferences!C14="P",1,(IF([1]Preferences!C14="N",0,(IF([1]Preferences!C14="U",-1,(IF([1]Preferences!C14="C",-1000)))))))</f>
+        <f>IF(Preferences!C14="P",1,(IF(Preferences!C14="N",0,(IF(Preferences!C14="U",-1,(IF(Preferences!C14="C",-1000)))))))</f>
         <v>1</v>
       </c>
       <c r="B4">
-        <f>IF([1]Preferences!D14="P",1,(IF([1]Preferences!D14="N",0,(IF([1]Preferences!D14="U",-1,(IF([1]Preferences!D14="C",-1000)))))))</f>
+        <f>IF(Preferences!D14="P",1,(IF(Preferences!D14="N",0,(IF(Preferences!D14="U",-1,(IF(Preferences!D14="C",-1000)))))))</f>
         <v>1</v>
       </c>
       <c r="C4">
-        <f>IF([1]Preferences!E14="P",1,(IF([1]Preferences!E14="N",0,(IF([1]Preferences!E14="U",-1,(IF([1]Preferences!E14="C",-1000)))))))</f>
+        <f>IF(Preferences!E14="P",1,(IF(Preferences!E14="N",0,(IF(Preferences!E14="U",-1,(IF(Preferences!E14="C",-1000)))))))</f>
         <v>1</v>
       </c>
       <c r="D4">
-        <f>IF([1]Preferences!F14="P",1,(IF([1]Preferences!F14="N",0,(IF([1]Preferences!F14="U",-1,(IF([1]Preferences!F14="C",-1000)))))))</f>
+        <f>IF(Preferences!F14="P",1,(IF(Preferences!F14="N",0,(IF(Preferences!F14="U",-1,(IF(Preferences!F14="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="E4">
-        <f>IF([1]Preferences!G14="P",1,(IF([1]Preferences!G14="N",0,(IF([1]Preferences!G14="U",-1,(IF([1]Preferences!G14="C",-1000)))))))</f>
+        <f>IF(Preferences!G14="P",1,(IF(Preferences!G14="N",0,(IF(Preferences!G14="U",-1,(IF(Preferences!G14="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="F4">
-        <f>IF([1]Preferences!H14="P",1,(IF([1]Preferences!H14="N",0,(IF([1]Preferences!H14="U",-1,(IF([1]Preferences!H14="C",-1000)))))))</f>
+        <f>IF(Preferences!H14="P",1,(IF(Preferences!H14="N",0,(IF(Preferences!H14="U",-1,(IF(Preferences!H14="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="G4">
-        <f>IF([1]Preferences!I14="P",1,(IF([1]Preferences!I14="N",0,(IF([1]Preferences!I14="U",-1,(IF([1]Preferences!I14="C",-1000)))))))</f>
+        <f>IF(Preferences!I14="P",1,(IF(Preferences!I14="N",0,(IF(Preferences!I14="U",-1,(IF(Preferences!I14="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="H4">
-        <f>IF([1]Preferences!J14="P",1,(IF([1]Preferences!J14="N",0,(IF([1]Preferences!J14="U",-1,(IF([1]Preferences!J14="C",-1000)))))))</f>
+        <f>IF(Preferences!J14="P",1,(IF(Preferences!J14="N",0,(IF(Preferences!J14="U",-1,(IF(Preferences!J14="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="I4">
-        <f>IF([1]Preferences!K14="P",1,(IF([1]Preferences!K14="N",0,(IF([1]Preferences!K14="U",-1,(IF([1]Preferences!K14="C",-1000)))))))</f>
+        <f>IF(Preferences!K14="P",1,(IF(Preferences!K14="N",0,(IF(Preferences!K14="U",-1,(IF(Preferences!K14="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="J4">
-        <f>IF([1]Preferences!L14="P",1,(IF([1]Preferences!L14="N",0,(IF([1]Preferences!L14="U",-1,(IF([1]Preferences!L14="C",-1000)))))))</f>
+        <f>IF(Preferences!L14="P",1,(IF(Preferences!L14="N",0,(IF(Preferences!L14="U",-1,(IF(Preferences!L14="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="K4">
-        <f>IF([1]Preferences!M14="P",1,(IF([1]Preferences!M14="N",0,(IF([1]Preferences!M14="U",-1,(IF([1]Preferences!M14="C",-1000)))))))</f>
+        <f>IF(Preferences!M14="P",1,(IF(Preferences!M14="N",0,(IF(Preferences!M14="U",-1,(IF(Preferences!M14="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="L4">
-        <f>IF([1]Preferences!N14="P",1,(IF([1]Preferences!N14="N",0,(IF([1]Preferences!N14="U",-1,(IF([1]Preferences!N14="C",-1000)))))))</f>
+        <f>IF(Preferences!N14="P",1,(IF(Preferences!N14="N",0,(IF(Preferences!N14="U",-1,(IF(Preferences!N14="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="M4">
-        <f>IF([1]Preferences!O14="P",1,(IF([1]Preferences!O14="N",0,(IF([1]Preferences!O14="U",-1,(IF([1]Preferences!O14="C",-1000)))))))</f>
+        <f>IF(Preferences!O14="P",1,(IF(Preferences!O14="N",0,(IF(Preferences!O14="U",-1,(IF(Preferences!O14="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="N4">
-        <f>IF([1]Preferences!P14="P",1,(IF([1]Preferences!P14="N",0,(IF([1]Preferences!P14="U",-1,(IF([1]Preferences!P14="C",-1000)))))))</f>
+        <f>IF(Preferences!P14="P",1,(IF(Preferences!P14="N",0,(IF(Preferences!P14="U",-1,(IF(Preferences!P14="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="O4">
-        <f>IF([1]Preferences!Q14="P",1,(IF([1]Preferences!Q14="N",0,(IF([1]Preferences!Q14="U",-1,(IF([1]Preferences!Q14="C",-1000)))))))</f>
+        <f>IF(Preferences!Q14="P",1,(IF(Preferences!Q14="N",0,(IF(Preferences!Q14="U",-1,(IF(Preferences!Q14="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="P4">
-        <f>IF([1]Preferences!R14="P",1,(IF([1]Preferences!R14="N",0,(IF([1]Preferences!R14="U",-1,(IF([1]Preferences!R14="C",-1000)))))))</f>
+        <f>IF(Preferences!R14="P",1,(IF(Preferences!R14="N",0,(IF(Preferences!R14="U",-1,(IF(Preferences!R14="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="Q4">
-        <f>IF([1]Preferences!S14="P",1,(IF([1]Preferences!S14="N",0,(IF([1]Preferences!S14="U",-1,(IF([1]Preferences!S14="C",-1000)))))))</f>
+        <f>IF(Preferences!S14="P",1,(IF(Preferences!S14="N",0,(IF(Preferences!S14="U",-1,(IF(Preferences!S14="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f>IF([1]Preferences!C15="P",1,(IF([1]Preferences!C15="N",0,(IF([1]Preferences!C15="U",-1,(IF([1]Preferences!C15="C",-1000)))))))</f>
+        <f>IF(Preferences!C15="P",1,(IF(Preferences!C15="N",0,(IF(Preferences!C15="U",-1,(IF(Preferences!C15="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="B5">
-        <f>IF([1]Preferences!D15="P",1,(IF([1]Preferences!D15="N",0,(IF([1]Preferences!D15="U",-1,(IF([1]Preferences!D15="C",-1000)))))))</f>
+        <f>IF(Preferences!D15="P",1,(IF(Preferences!D15="N",0,(IF(Preferences!D15="U",-1,(IF(Preferences!D15="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="C5">
-        <f>IF([1]Preferences!E15="P",1,(IF([1]Preferences!E15="N",0,(IF([1]Preferences!E15="U",-1,(IF([1]Preferences!E15="C",-1000)))))))</f>
+        <f>IF(Preferences!E15="P",1,(IF(Preferences!E15="N",0,(IF(Preferences!E15="U",-1,(IF(Preferences!E15="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="D5">
-        <f>IF([1]Preferences!F15="P",1,(IF([1]Preferences!F15="N",0,(IF([1]Preferences!F15="U",-1,(IF([1]Preferences!F15="C",-1000)))))))</f>
+        <f>IF(Preferences!F15="P",1,(IF(Preferences!F15="N",0,(IF(Preferences!F15="U",-1,(IF(Preferences!F15="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="E5">
-        <f>IF([1]Preferences!G15="P",1,(IF([1]Preferences!G15="N",0,(IF([1]Preferences!G15="U",-1,(IF([1]Preferences!G15="C",-1000)))))))</f>
+        <f>IF(Preferences!G15="P",1,(IF(Preferences!G15="N",0,(IF(Preferences!G15="U",-1,(IF(Preferences!G15="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="F5">
-        <f>IF([1]Preferences!H15="P",1,(IF([1]Preferences!H15="N",0,(IF([1]Preferences!H15="U",-1,(IF([1]Preferences!H15="C",-1000)))))))</f>
+        <f>IF(Preferences!H15="P",1,(IF(Preferences!H15="N",0,(IF(Preferences!H15="U",-1,(IF(Preferences!H15="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="G5">
-        <f>IF([1]Preferences!I15="P",1,(IF([1]Preferences!I15="N",0,(IF([1]Preferences!I15="U",-1,(IF([1]Preferences!I15="C",-1000)))))))</f>
+        <f>IF(Preferences!I15="P",1,(IF(Preferences!I15="N",0,(IF(Preferences!I15="U",-1,(IF(Preferences!I15="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="H5">
-        <f>IF([1]Preferences!J15="P",1,(IF([1]Preferences!J15="N",0,(IF([1]Preferences!J15="U",-1,(IF([1]Preferences!J15="C",-1000)))))))</f>
+        <f>IF(Preferences!J15="P",1,(IF(Preferences!J15="N",0,(IF(Preferences!J15="U",-1,(IF(Preferences!J15="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="I5">
-        <f>IF([1]Preferences!K15="P",1,(IF([1]Preferences!K15="N",0,(IF([1]Preferences!K15="U",-1,(IF([1]Preferences!K15="C",-1000)))))))</f>
+        <f>IF(Preferences!K15="P",1,(IF(Preferences!K15="N",0,(IF(Preferences!K15="U",-1,(IF(Preferences!K15="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="J5">
-        <f>IF([1]Preferences!L15="P",1,(IF([1]Preferences!L15="N",0,(IF([1]Preferences!L15="U",-1,(IF([1]Preferences!L15="C",-1000)))))))</f>
+        <f>IF(Preferences!L15="P",1,(IF(Preferences!L15="N",0,(IF(Preferences!L15="U",-1,(IF(Preferences!L15="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="K5">
-        <f>IF([1]Preferences!M15="P",1,(IF([1]Preferences!M15="N",0,(IF([1]Preferences!M15="U",-1,(IF([1]Preferences!M15="C",-1000)))))))</f>
+        <f>IF(Preferences!M15="P",1,(IF(Preferences!M15="N",0,(IF(Preferences!M15="U",-1,(IF(Preferences!M15="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="L5">
-        <f>IF([1]Preferences!N15="P",1,(IF([1]Preferences!N15="N",0,(IF([1]Preferences!N15="U",-1,(IF([1]Preferences!N15="C",-1000)))))))</f>
+        <f>IF(Preferences!N15="P",1,(IF(Preferences!N15="N",0,(IF(Preferences!N15="U",-1,(IF(Preferences!N15="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="M5">
-        <f>IF([1]Preferences!O15="P",1,(IF([1]Preferences!O15="N",0,(IF([1]Preferences!O15="U",-1,(IF([1]Preferences!O15="C",-1000)))))))</f>
+        <f>IF(Preferences!O15="P",1,(IF(Preferences!O15="N",0,(IF(Preferences!O15="U",-1,(IF(Preferences!O15="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="N5">
-        <f>IF([1]Preferences!P15="P",1,(IF([1]Preferences!P15="N",0,(IF([1]Preferences!P15="U",-1,(IF([1]Preferences!P15="C",-1000)))))))</f>
+        <f>IF(Preferences!P15="P",1,(IF(Preferences!P15="N",0,(IF(Preferences!P15="U",-1,(IF(Preferences!P15="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="O5">
-        <f>IF([1]Preferences!Q15="P",1,(IF([1]Preferences!Q15="N",0,(IF([1]Preferences!Q15="U",-1,(IF([1]Preferences!Q15="C",-1000)))))))</f>
+        <f>IF(Preferences!Q15="P",1,(IF(Preferences!Q15="N",0,(IF(Preferences!Q15="U",-1,(IF(Preferences!Q15="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="P5">
-        <f>IF([1]Preferences!R15="P",1,(IF([1]Preferences!R15="N",0,(IF([1]Preferences!R15="U",-1,(IF([1]Preferences!R15="C",-1000)))))))</f>
+        <f>IF(Preferences!R15="P",1,(IF(Preferences!R15="N",0,(IF(Preferences!R15="U",-1,(IF(Preferences!R15="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="Q5">
-        <f>IF([1]Preferences!S15="P",1,(IF([1]Preferences!S15="N",0,(IF([1]Preferences!S15="U",-1,(IF([1]Preferences!S15="C",-1000)))))))</f>
+        <f>IF(Preferences!S15="P",1,(IF(Preferences!S15="N",0,(IF(Preferences!S15="U",-1,(IF(Preferences!S15="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f>IF([1]Preferences!C16="P",1,(IF([1]Preferences!C16="N",0,(IF([1]Preferences!C16="U",-1,(IF([1]Preferences!C16="C",-1000)))))))</f>
+        <f>IF(Preferences!C16="P",1,(IF(Preferences!C16="N",0,(IF(Preferences!C16="U",-1,(IF(Preferences!C16="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="B6">
-        <f>IF([1]Preferences!D16="P",1,(IF([1]Preferences!D16="N",0,(IF([1]Preferences!D16="U",-1,(IF([1]Preferences!D16="C",-1000)))))))</f>
+        <f>IF(Preferences!D16="P",1,(IF(Preferences!D16="N",0,(IF(Preferences!D16="U",-1,(IF(Preferences!D16="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="C6">
-        <f>IF([1]Preferences!E16="P",1,(IF([1]Preferences!E16="N",0,(IF([1]Preferences!E16="U",-1,(IF([1]Preferences!E16="C",-1000)))))))</f>
+        <f>IF(Preferences!E16="P",1,(IF(Preferences!E16="N",0,(IF(Preferences!E16="U",-1,(IF(Preferences!E16="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="D6">
-        <f>IF([1]Preferences!F16="P",1,(IF([1]Preferences!F16="N",0,(IF([1]Preferences!F16="U",-1,(IF([1]Preferences!F16="C",-1000)))))))</f>
+        <f>IF(Preferences!F16="P",1,(IF(Preferences!F16="N",0,(IF(Preferences!F16="U",-1,(IF(Preferences!F16="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="E6">
-        <f>IF([1]Preferences!G16="P",1,(IF([1]Preferences!G16="N",0,(IF([1]Preferences!G16="U",-1,(IF([1]Preferences!G16="C",-1000)))))))</f>
+        <f>IF(Preferences!G16="P",1,(IF(Preferences!G16="N",0,(IF(Preferences!G16="U",-1,(IF(Preferences!G16="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="F6">
-        <f>IF([1]Preferences!H16="P",1,(IF([1]Preferences!H16="N",0,(IF([1]Preferences!H16="U",-1,(IF([1]Preferences!H16="C",-1000)))))))</f>
+        <f>IF(Preferences!H16="P",1,(IF(Preferences!H16="N",0,(IF(Preferences!H16="U",-1,(IF(Preferences!H16="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="G6">
-        <f>IF([1]Preferences!I16="P",1,(IF([1]Preferences!I16="N",0,(IF([1]Preferences!I16="U",-1,(IF([1]Preferences!I16="C",-1000)))))))</f>
+        <f>IF(Preferences!I16="P",1,(IF(Preferences!I16="N",0,(IF(Preferences!I16="U",-1,(IF(Preferences!I16="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="H6">
-        <f>IF([1]Preferences!J16="P",1,(IF([1]Preferences!J16="N",0,(IF([1]Preferences!J16="U",-1,(IF([1]Preferences!J16="C",-1000)))))))</f>
+        <f>IF(Preferences!J16="P",1,(IF(Preferences!J16="N",0,(IF(Preferences!J16="U",-1,(IF(Preferences!J16="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="I6">
-        <f>IF([1]Preferences!K16="P",1,(IF([1]Preferences!K16="N",0,(IF([1]Preferences!K16="U",-1,(IF([1]Preferences!K16="C",-1000)))))))</f>
+        <f>IF(Preferences!K16="P",1,(IF(Preferences!K16="N",0,(IF(Preferences!K16="U",-1,(IF(Preferences!K16="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="J6">
-        <f>IF([1]Preferences!L16="P",1,(IF([1]Preferences!L16="N",0,(IF([1]Preferences!L16="U",-1,(IF([1]Preferences!L16="C",-1000)))))))</f>
+        <f>IF(Preferences!L16="P",1,(IF(Preferences!L16="N",0,(IF(Preferences!L16="U",-1,(IF(Preferences!L16="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="K6">
-        <f>IF([1]Preferences!M16="P",1,(IF([1]Preferences!M16="N",0,(IF([1]Preferences!M16="U",-1,(IF([1]Preferences!M16="C",-1000)))))))</f>
+        <f>IF(Preferences!M16="P",1,(IF(Preferences!M16="N",0,(IF(Preferences!M16="U",-1,(IF(Preferences!M16="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="L6">
-        <f>IF([1]Preferences!N16="P",1,(IF([1]Preferences!N16="N",0,(IF([1]Preferences!N16="U",-1,(IF([1]Preferences!N16="C",-1000)))))))</f>
+        <f>IF(Preferences!N16="P",1,(IF(Preferences!N16="N",0,(IF(Preferences!N16="U",-1,(IF(Preferences!N16="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="M6">
-        <f>IF([1]Preferences!O16="P",1,(IF([1]Preferences!O16="N",0,(IF([1]Preferences!O16="U",-1,(IF([1]Preferences!O16="C",-1000)))))))</f>
+        <f>IF(Preferences!O16="P",1,(IF(Preferences!O16="N",0,(IF(Preferences!O16="U",-1,(IF(Preferences!O16="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="N6">
-        <f>IF([1]Preferences!P16="P",1,(IF([1]Preferences!P16="N",0,(IF([1]Preferences!P16="U",-1,(IF([1]Preferences!P16="C",-1000)))))))</f>
+        <f>IF(Preferences!P16="P",1,(IF(Preferences!P16="N",0,(IF(Preferences!P16="U",-1,(IF(Preferences!P16="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="O6">
-        <f>IF([1]Preferences!Q16="P",1,(IF([1]Preferences!Q16="N",0,(IF([1]Preferences!Q16="U",-1,(IF([1]Preferences!Q16="C",-1000)))))))</f>
+        <f>IF(Preferences!Q16="P",1,(IF(Preferences!Q16="N",0,(IF(Preferences!Q16="U",-1,(IF(Preferences!Q16="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="P6">
-        <f>IF([1]Preferences!R16="P",1,(IF([1]Preferences!R16="N",0,(IF([1]Preferences!R16="U",-1,(IF([1]Preferences!R16="C",-1000)))))))</f>
+        <f>IF(Preferences!R16="P",1,(IF(Preferences!R16="N",0,(IF(Preferences!R16="U",-1,(IF(Preferences!R16="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="Q6">
-        <f>IF([1]Preferences!S16="P",1,(IF([1]Preferences!S16="N",0,(IF([1]Preferences!S16="U",-1,(IF([1]Preferences!S16="C",-1000)))))))</f>
+        <f>IF(Preferences!S16="P",1,(IF(Preferences!S16="N",0,(IF(Preferences!S16="U",-1,(IF(Preferences!S16="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f>IF([1]Preferences!C17="P",1,(IF([1]Preferences!C17="N",0,(IF([1]Preferences!C17="U",-1,(IF([1]Preferences!C17="C",-1000)))))))</f>
+        <f>IF(Preferences!C17="P",1,(IF(Preferences!C17="N",0,(IF(Preferences!C17="U",-1,(IF(Preferences!C17="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="B7">
-        <f>IF([1]Preferences!D17="P",1,(IF([1]Preferences!D17="N",0,(IF([1]Preferences!D17="U",-1,(IF([1]Preferences!D17="C",-1000)))))))</f>
+        <f>IF(Preferences!D17="P",1,(IF(Preferences!D17="N",0,(IF(Preferences!D17="U",-1,(IF(Preferences!D17="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="C7">
-        <f>IF([1]Preferences!E17="P",1,(IF([1]Preferences!E17="N",0,(IF([1]Preferences!E17="U",-1,(IF([1]Preferences!E17="C",-1000)))))))</f>
+        <f>IF(Preferences!E17="P",1,(IF(Preferences!E17="N",0,(IF(Preferences!E17="U",-1,(IF(Preferences!E17="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="D7">
-        <f>IF([1]Preferences!F17="P",1,(IF([1]Preferences!F17="N",0,(IF([1]Preferences!F17="U",-1,(IF([1]Preferences!F17="C",-1000)))))))</f>
+        <f>IF(Preferences!F17="P",1,(IF(Preferences!F17="N",0,(IF(Preferences!F17="U",-1,(IF(Preferences!F17="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="E7">
-        <f>IF([1]Preferences!G17="P",1,(IF([1]Preferences!G17="N",0,(IF([1]Preferences!G17="U",-1,(IF([1]Preferences!G17="C",-1000)))))))</f>
+        <f>IF(Preferences!G17="P",1,(IF(Preferences!G17="N",0,(IF(Preferences!G17="U",-1,(IF(Preferences!G17="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="F7">
-        <f>IF([1]Preferences!H17="P",1,(IF([1]Preferences!H17="N",0,(IF([1]Preferences!H17="U",-1,(IF([1]Preferences!H17="C",-1000)))))))</f>
+        <f>IF(Preferences!H17="P",1,(IF(Preferences!H17="N",0,(IF(Preferences!H17="U",-1,(IF(Preferences!H17="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="G7">
-        <f>IF([1]Preferences!I17="P",1,(IF([1]Preferences!I17="N",0,(IF([1]Preferences!I17="U",-1,(IF([1]Preferences!I17="C",-1000)))))))</f>
+        <f>IF(Preferences!I17="P",1,(IF(Preferences!I17="N",0,(IF(Preferences!I17="U",-1,(IF(Preferences!I17="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="H7">
-        <f>IF([1]Preferences!J17="P",1,(IF([1]Preferences!J17="N",0,(IF([1]Preferences!J17="U",-1,(IF([1]Preferences!J17="C",-1000)))))))</f>
+        <f>IF(Preferences!J17="P",1,(IF(Preferences!J17="N",0,(IF(Preferences!J17="U",-1,(IF(Preferences!J17="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="I7">
-        <f>IF([1]Preferences!K17="P",1,(IF([1]Preferences!K17="N",0,(IF([1]Preferences!K17="U",-1,(IF([1]Preferences!K17="C",-1000)))))))</f>
+        <f>IF(Preferences!K17="P",1,(IF(Preferences!K17="N",0,(IF(Preferences!K17="U",-1,(IF(Preferences!K17="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="J7">
-        <f>IF([1]Preferences!L17="P",1,(IF([1]Preferences!L17="N",0,(IF([1]Preferences!L17="U",-1,(IF([1]Preferences!L17="C",-1000)))))))</f>
+        <f>IF(Preferences!L17="P",1,(IF(Preferences!L17="N",0,(IF(Preferences!L17="U",-1,(IF(Preferences!L17="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="K7">
-        <f>IF([1]Preferences!M17="P",1,(IF([1]Preferences!M17="N",0,(IF([1]Preferences!M17="U",-1,(IF([1]Preferences!M17="C",-1000)))))))</f>
+        <f>IF(Preferences!M17="P",1,(IF(Preferences!M17="N",0,(IF(Preferences!M17="U",-1,(IF(Preferences!M17="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="L7">
-        <f>IF([1]Preferences!N17="P",1,(IF([1]Preferences!N17="N",0,(IF([1]Preferences!N17="U",-1,(IF([1]Preferences!N17="C",-1000)))))))</f>
+        <f>IF(Preferences!N17="P",1,(IF(Preferences!N17="N",0,(IF(Preferences!N17="U",-1,(IF(Preferences!N17="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="M7">
-        <f>IF([1]Preferences!O17="P",1,(IF([1]Preferences!O17="N",0,(IF([1]Preferences!O17="U",-1,(IF([1]Preferences!O17="C",-1000)))))))</f>
+        <f>IF(Preferences!O17="P",1,(IF(Preferences!O17="N",0,(IF(Preferences!O17="U",-1,(IF(Preferences!O17="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="N7">
-        <f>IF([1]Preferences!P17="P",1,(IF([1]Preferences!P17="N",0,(IF([1]Preferences!P17="U",-1,(IF([1]Preferences!P17="C",-1000)))))))</f>
+        <f>IF(Preferences!P17="P",1,(IF(Preferences!P17="N",0,(IF(Preferences!P17="U",-1,(IF(Preferences!P17="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="O7">
-        <f>IF([1]Preferences!Q17="P",1,(IF([1]Preferences!Q17="N",0,(IF([1]Preferences!Q17="U",-1,(IF([1]Preferences!Q17="C",-1000)))))))</f>
+        <f>IF(Preferences!Q17="P",1,(IF(Preferences!Q17="N",0,(IF(Preferences!Q17="U",-1,(IF(Preferences!Q17="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="P7">
-        <f>IF([1]Preferences!R17="P",1,(IF([1]Preferences!R17="N",0,(IF([1]Preferences!R17="U",-1,(IF([1]Preferences!R17="C",-1000)))))))</f>
+        <f>IF(Preferences!R17="P",1,(IF(Preferences!R17="N",0,(IF(Preferences!R17="U",-1,(IF(Preferences!R17="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="Q7">
-        <f>IF([1]Preferences!S17="P",1,(IF([1]Preferences!S17="N",0,(IF([1]Preferences!S17="U",-1,(IF([1]Preferences!S17="C",-1000)))))))</f>
+        <f>IF(Preferences!S17="P",1,(IF(Preferences!S17="N",0,(IF(Preferences!S17="U",-1,(IF(Preferences!S17="C",-1000)))))))</f>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f>IF([1]Preferences!C18="P",1,(IF([1]Preferences!C18="N",0,(IF([1]Preferences!C18="U",-1,(IF([1]Preferences!C18="C",-1000)))))))</f>
+        <f>IF(Preferences!C18="P",1,(IF(Preferences!C18="N",0,(IF(Preferences!C18="U",-1,(IF(Preferences!C18="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="B8">
-        <f>IF([1]Preferences!D18="P",1,(IF([1]Preferences!D18="N",0,(IF([1]Preferences!D18="U",-1,(IF([1]Preferences!D18="C",-1000)))))))</f>
+        <f>IF(Preferences!D18="P",1,(IF(Preferences!D18="N",0,(IF(Preferences!D18="U",-1,(IF(Preferences!D18="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="C8">
-        <f>IF([1]Preferences!E18="P",1,(IF([1]Preferences!E18="N",0,(IF([1]Preferences!E18="U",-1,(IF([1]Preferences!E18="C",-1000)))))))</f>
+        <f>IF(Preferences!E18="P",1,(IF(Preferences!E18="N",0,(IF(Preferences!E18="U",-1,(IF(Preferences!E18="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="D8">
-        <f>IF([1]Preferences!F18="P",1,(IF([1]Preferences!F18="N",0,(IF([1]Preferences!F18="U",-1,(IF([1]Preferences!F18="C",-1000)))))))</f>
+        <f>IF(Preferences!F18="P",1,(IF(Preferences!F18="N",0,(IF(Preferences!F18="U",-1,(IF(Preferences!F18="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="E8">
-        <f>IF([1]Preferences!G18="P",1,(IF([1]Preferences!G18="N",0,(IF([1]Preferences!G18="U",-1,(IF([1]Preferences!G18="C",-1000)))))))</f>
+        <f>IF(Preferences!G18="P",1,(IF(Preferences!G18="N",0,(IF(Preferences!G18="U",-1,(IF(Preferences!G18="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="F8">
-        <f>IF([1]Preferences!H18="P",1,(IF([1]Preferences!H18="N",0,(IF([1]Preferences!H18="U",-1,(IF([1]Preferences!H18="C",-1000)))))))</f>
+        <f>IF(Preferences!H18="P",1,(IF(Preferences!H18="N",0,(IF(Preferences!H18="U",-1,(IF(Preferences!H18="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="G8">
-        <f>IF([1]Preferences!I18="P",1,(IF([1]Preferences!I18="N",0,(IF([1]Preferences!I18="U",-1,(IF([1]Preferences!I18="C",-1000)))))))</f>
+        <f>IF(Preferences!I18="P",1,(IF(Preferences!I18="N",0,(IF(Preferences!I18="U",-1,(IF(Preferences!I18="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="H8">
-        <f>IF([1]Preferences!J18="P",1,(IF([1]Preferences!J18="N",0,(IF([1]Preferences!J18="U",-1,(IF([1]Preferences!J18="C",-1000)))))))</f>
+        <f>IF(Preferences!J18="P",1,(IF(Preferences!J18="N",0,(IF(Preferences!J18="U",-1,(IF(Preferences!J18="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="I8">
-        <f>IF([1]Preferences!K18="P",1,(IF([1]Preferences!K18="N",0,(IF([1]Preferences!K18="U",-1,(IF([1]Preferences!K18="C",-1000)))))))</f>
+        <f>IF(Preferences!K18="P",1,(IF(Preferences!K18="N",0,(IF(Preferences!K18="U",-1,(IF(Preferences!K18="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="J8">
-        <f>IF([1]Preferences!L18="P",1,(IF([1]Preferences!L18="N",0,(IF([1]Preferences!L18="U",-1,(IF([1]Preferences!L18="C",-1000)))))))</f>
+        <f>IF(Preferences!L18="P",1,(IF(Preferences!L18="N",0,(IF(Preferences!L18="U",-1,(IF(Preferences!L18="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="K8">
-        <f>IF([1]Preferences!M18="P",1,(IF([1]Preferences!M18="N",0,(IF([1]Preferences!M18="U",-1,(IF([1]Preferences!M18="C",-1000)))))))</f>
+        <f>IF(Preferences!M18="P",1,(IF(Preferences!M18="N",0,(IF(Preferences!M18="U",-1,(IF(Preferences!M18="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="L8">
-        <f>IF([1]Preferences!N18="P",1,(IF([1]Preferences!N18="N",0,(IF([1]Preferences!N18="U",-1,(IF([1]Preferences!N18="C",-1000)))))))</f>
+        <f>IF(Preferences!N18="P",1,(IF(Preferences!N18="N",0,(IF(Preferences!N18="U",-1,(IF(Preferences!N18="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="M8">
-        <f>IF([1]Preferences!O18="P",1,(IF([1]Preferences!O18="N",0,(IF([1]Preferences!O18="U",-1,(IF([1]Preferences!O18="C",-1000)))))))</f>
+        <f>IF(Preferences!O18="P",1,(IF(Preferences!O18="N",0,(IF(Preferences!O18="U",-1,(IF(Preferences!O18="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="N8">
-        <f>IF([1]Preferences!P18="P",1,(IF([1]Preferences!P18="N",0,(IF([1]Preferences!P18="U",-1,(IF([1]Preferences!P18="C",-1000)))))))</f>
+        <f>IF(Preferences!P18="P",1,(IF(Preferences!P18="N",0,(IF(Preferences!P18="U",-1,(IF(Preferences!P18="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="O8">
-        <f>IF([1]Preferences!Q18="P",1,(IF([1]Preferences!Q18="N",0,(IF([1]Preferences!Q18="U",-1,(IF([1]Preferences!Q18="C",-1000)))))))</f>
+        <f>IF(Preferences!Q18="P",1,(IF(Preferences!Q18="N",0,(IF(Preferences!Q18="U",-1,(IF(Preferences!Q18="C",-1000)))))))</f>
         <v>0</v>
       </c>
       <c r="P8">
-        <f>IF([1]Preferences!R18="P",1,(IF([1]Preferences!R18="N",0,(IF([1]Preferences!R18="U",-1,(IF([1]Preferences!R18="C",-1000)))))))</f>
+        <f>IF(Preferences!R18="P",1,(IF(Preferences!R18="N",0,(IF(Preferences!R18="U",-1,(IF(Preferences!R18="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
       <c r="Q8">
-        <f>IF([1]Preferences!S18="P",1,(IF([1]Preferences!S18="N",0,(IF([1]Preferences!S18="U",-1,(IF([1]Preferences!S18="C",-1000)))))))</f>
+        <f>IF(Preferences!S18="P",1,(IF(Preferences!S18="N",0,(IF(Preferences!S18="U",-1,(IF(Preferences!S18="C",-1000)))))))</f>
         <v>-1000</v>
       </c>
     </row>
@@ -3144,7 +2699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D9FE1CB-E762-4D98-9A11-E2BCA04378C5}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
@@ -3157,7 +2712,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3540,7 +3095,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
no more camel case
</commit_message>
<xml_diff>
--- a/table.xlsx
+++ b/table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Desktop\GitHub\spl-schedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8014A6B4-802F-4EDF-8373-92B379157BBA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFDC37DC-C93D-4647-94C5-8D01CC1EBF28}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CB2829CA-F4A0-41C5-B1C7-1ACBB28571D8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{CB2829CA-F4A0-41C5-B1C7-1ACBB28571D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Preferences" sheetId="1" r:id="rId1"/>
@@ -2102,7 +2102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1377A6A-D636-40DB-9A3C-30FAF9FA189C}">
   <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="72" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
@@ -3907,7 +3907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B873E99C-54D7-42F4-80D7-7C19170AA59C}">
   <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView zoomScale="66" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>

</xml_diff>